<commit_message>
fix import employeeSMD Pasar dll
</commit_message>
<xml_diff>
--- a/public/assets/EmployeeSmdImport.xlsx
+++ b/public/assets/EmployeeSmdImport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\sasa_mtcgtc\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>dsaad</t>
-  </si>
-  <si>
-    <t>dasd</t>
-  </si>
-  <si>
-    <t>yweqe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>SD</t>
   </si>
@@ -45,12 +36,6 @@
     <t>BCA</t>
   </si>
   <si>
-    <t>ddada@gamil.com</t>
-  </si>
-  <si>
-    <t>Dada</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -103,13 +88,52 @@
   </si>
   <si>
     <t>NIK</t>
+  </si>
+  <si>
+    <t>WITA</t>
+  </si>
+  <si>
+    <t>region123</t>
+  </si>
+  <si>
+    <t>area124</t>
+  </si>
+  <si>
+    <t>subarea456</t>
+  </si>
+  <si>
+    <t>sada@gmail.com</t>
+  </si>
+  <si>
+    <t>Sada123</t>
+  </si>
+  <si>
+    <t>Sada12345</t>
+  </si>
+  <si>
+    <t>sada123@gmail.com</t>
+  </si>
+  <si>
+    <t>WIB</t>
+  </si>
+  <si>
+    <t>baru2</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>Baru4, baru5</t>
+  </si>
+  <si>
+    <t>area1245</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -120,6 +144,13 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,10 +174,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -431,122 +466,167 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>12334</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>123456</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
-        <v>21324234</v>
+        <v>218884411</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G2" s="1">
         <v>12141</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>6</v>
+      <c r="J2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="O2" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12345</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>8889996</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>